<commit_message>
Doc of LocoBufer Cradle
</commit_message>
<xml_diff>
--- a/Interfaces/LocoBufferEsp32/board/LocoBufferEsp32Craddle/doc/LocoBuffer-bom.xlsx
+++ b/Interfaces/LocoBufferEsp32/board/LocoBufferEsp32Craddle/doc/LocoBuffer-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="143">
   <si>
     <t>Row</t>
   </si>
@@ -110,6 +110,24 @@
     <t>3</t>
   </si>
   <si>
+    <t>RGB LED, red/green/blue/anode</t>
+  </si>
+  <si>
+    <t>LED_RGBA</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>LTST-C19HE1WT</t>
+  </si>
+  <si>
+    <t>LED_LiteOn_LTST-C19HE1WT</t>
+  </si>
+  <si>
+    <t>C458749</t>
+  </si>
+  <si>
     <t>Diode</t>
   </si>
   <si>
@@ -131,6 +149,9 @@
     <t>1=K 2=A</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>Generic connector, single row, 01x04, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -143,7 +164,7 @@
     <t>PinHeader_1x04_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t>5</t>
+    <t>6</t>
   </si>
   <si>
     <t>RJ connector, 6P6C (6 positions 6 connected)</t>
@@ -158,7 +179,7 @@
     <t>AMPHENOL_RJE0166001</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>NPN transistor, base/emitter/collector</t>
@@ -179,7 +200,7 @@
     <t>C2150</t>
   </si>
   <si>
-    <t>7</t>
+    <t>8</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -200,10 +221,10 @@
     <t>C17714</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>R6 R8 R12 R13</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>R6 R8 R12 R13 R14 R15 R16</t>
   </si>
   <si>
     <t>470</t>
@@ -212,7 +233,7 @@
     <t>C17710</t>
   </si>
   <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>R3</t>
@@ -224,7 +245,7 @@
     <t>C17513</t>
   </si>
   <si>
-    <t>10</t>
+    <t>11</t>
   </si>
   <si>
     <t>R9 R11</t>
@@ -236,7 +257,7 @@
     <t>C229219</t>
   </si>
   <si>
-    <t>11</t>
+    <t>12</t>
   </si>
   <si>
     <t>R2</t>
@@ -248,7 +269,7 @@
     <t>C17560</t>
   </si>
   <si>
-    <t>12</t>
+    <t>13</t>
   </si>
   <si>
     <t>R4</t>
@@ -260,7 +281,7 @@
     <t>C17713</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>R5</t>
@@ -272,7 +293,7 @@
     <t>C17470</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
   <si>
     <t>R7</t>
@@ -284,10 +305,10 @@
     <t>C17556</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>R1</t>
+    <t>16</t>
+  </si>
+  <si>
+    <t>R1 R17</t>
   </si>
   <si>
     <t>10K (5%)</t>
@@ -296,7 +317,22 @@
     <t>C17414</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Push button switch, generic, two pins</t>
+  </si>
+  <si>
+    <t>SW_Push</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SW_SPST_CK_RS282G05A3</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
   <si>
     <t>1A Low Dropout regulator, positive, 5.0V fixed output, SOT-223</t>
@@ -317,7 +353,7 @@
     <t>C6187</t>
   </si>
   <si>
-    <t>17</t>
+    <t>19</t>
   </si>
   <si>
     <t>Development Kit</t>
@@ -332,7 +368,7 @@
     <t>https://docs.espressif.com/projects/esp-idf/zh_CN/latest/esp32/hw-reference/esp32/get-started-devkitc.html</t>
   </si>
   <si>
-    <t>18</t>
+    <t>20</t>
   </si>
   <si>
     <t>Voltage Comparator, DIP-8/SOIC-8</t>
@@ -374,7 +410,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-07-10_07-56-20</t>
+    <t>2023-07-16_18-33-25</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -389,7 +425,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>30 (26 SMD/ 4 THT)</t>
+    <t>36 (32 SMD/ 4 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -907,7 +943,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -932,7 +968,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -946,55 +982,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="F2" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1002,16 +1038,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="F6" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1148,7 +1184,7 @@
         <v>34</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>19</v>
@@ -1159,34 +1195,34 @@
       <c r="J11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30" customHeight="1">
+      <c r="K11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>40</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>19</v>
@@ -1194,37 +1230,37 @@
       <c r="I12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="J12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>19</v>
@@ -1244,22 +1280,22 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>18</v>
@@ -1270,8 +1306,8 @@
       <c r="I14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="10" t="s">
-        <v>52</v>
+      <c r="J14" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>22</v>
@@ -1300,7 +1336,7 @@
         <v>58</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>19</v>
@@ -1323,22 +1359,22 @@
         <v>60</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>19</v>
@@ -1347,7 +1383,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>22</v>
@@ -1358,25 +1394,25 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="G17" s="5" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>19</v>
@@ -1385,7 +1421,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>22</v>
@@ -1396,25 +1432,25 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>19</v>
@@ -1423,7 +1459,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>22</v>
@@ -1434,25 +1470,25 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>19</v>
@@ -1461,7 +1497,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>22</v>
@@ -1472,22 +1508,22 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>12</v>
@@ -1499,7 +1535,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>22</v>
@@ -1510,22 +1546,22 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>12</v>
@@ -1537,7 +1573,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>22</v>
@@ -1548,22 +1584,22 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="9" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>12</v>
@@ -1575,7 +1611,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>22</v>
@@ -1586,22 +1622,22 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>12</v>
@@ -1613,7 +1649,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>22</v>
@@ -1622,33 +1658,33 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="30" customHeight="1">
+    <row r="24" spans="1:12">
       <c r="A24" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="11" t="s">
-        <v>97</v>
+      <c r="I24" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="J24" s="10" t="s">
         <v>98</v>
@@ -1660,7 +1696,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="45" customHeight="1">
+    <row r="25" spans="1:12">
       <c r="A25" s="5" t="s">
         <v>99</v>
       </c>
@@ -1677,7 +1713,7 @@
         <v>101</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>12</v>
@@ -1685,8 +1721,8 @@
       <c r="H25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>103</v>
+      <c r="I25" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>22</v>
@@ -1698,7 +1734,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
         <v>104</v>
       </c>
@@ -1733,6 +1769,82 @@
         <v>22</v>
       </c>
       <c r="L26" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="45" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1759,22 +1871,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SVG for LocoBuffer Esp32
</commit_message>
<xml_diff>
--- a/Interfaces/LocoBufferEsp32/board/LocoBufferEsp32Craddle/doc/LocoBuffer-bom.xlsx
+++ b/Interfaces/LocoBufferEsp32/board/LocoBufferEsp32Craddle/doc/LocoBuffer-bom.xlsx
@@ -419,7 +419,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>7.0.2.1-36-g582732918d-dirty-deb11</t>
+    <t>7.0.5.1-1-g8f565ef7f0-dirty-deb11</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -958,7 +958,7 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>

</xml_diff>